<commit_message>
por si las dudas
</commit_message>
<xml_diff>
--- a/Crossword_examen_1.xlsx
+++ b/Crossword_examen_1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/a01274912/Documents/DAW/A01274912ExaPar1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DC8A710-46FD-C54F-91FC-9EA01FEFF3C7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCDE5DCF-8679-2A4D-BE93-67EA12AE4C54}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="51200" windowHeight="26740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="58">
   <si>
     <t>HORIZONTAL</t>
   </si>
@@ -188,6 +188,12 @@
   </si>
   <si>
     <t>f</t>
+  </si>
+  <si>
+    <t>q</t>
+  </si>
+  <si>
+    <t>business</t>
   </si>
 </sst>
 </file>
@@ -644,10 +650,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="B2:AL55"/>
+  <dimension ref="B2:AR55"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P11" sqref="P11"/>
+      <selection activeCell="K9" sqref="K9:Q9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -772,7 +778,9 @@
       <c r="AC4" s="7"/>
       <c r="AD4" s="7"/>
       <c r="AE4" s="5"/>
-      <c r="AF4" s="5"/>
+      <c r="AF4" s="5" t="s">
+        <v>36</v>
+      </c>
       <c r="AG4" s="1"/>
       <c r="AH4" s="1"/>
       <c r="AI4" s="1"/>
@@ -805,17 +813,33 @@
       <c r="W5" s="8">
         <v>4</v>
       </c>
-      <c r="X5" s="5"/>
+      <c r="X5" s="5" t="s">
+        <v>45</v>
+      </c>
       <c r="Y5" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="Z5" s="5"/>
-      <c r="AA5" s="5"/>
-      <c r="AB5" s="5"/>
-      <c r="AC5" s="5"/>
-      <c r="AD5" s="5"/>
-      <c r="AE5" s="5"/>
-      <c r="AF5" s="5"/>
+      <c r="Z5" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="AA5" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="AB5" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="AC5" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="AD5" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="AE5" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="AF5" s="5" t="s">
+        <v>35</v>
+      </c>
       <c r="AG5" s="1"/>
       <c r="AH5" s="1"/>
       <c r="AI5" s="1"/>
@@ -858,7 +882,9 @@
       <c r="AC6" s="1"/>
       <c r="AD6" s="1"/>
       <c r="AE6" s="4"/>
-      <c r="AF6" s="5"/>
+      <c r="AF6" s="5" t="s">
+        <v>27</v>
+      </c>
       <c r="AG6" s="1"/>
       <c r="AH6" s="1"/>
       <c r="AI6" s="4"/>
@@ -903,7 +929,9 @@
         <v>6</v>
       </c>
       <c r="AE7" s="4"/>
-      <c r="AF7" s="5"/>
+      <c r="AF7" s="5" t="s">
+        <v>36</v>
+      </c>
       <c r="AG7" s="7"/>
       <c r="AH7" s="7"/>
       <c r="AI7" s="5"/>
@@ -955,22 +983,22 @@
         <v>7</v>
       </c>
       <c r="AF8" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="AG8" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="AH8" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="AI8" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="AG8" s="5" t="s">
+      <c r="AJ8" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="AH8" s="5" t="s">
+      <c r="AK8" s="5" t="s">
         <v>54</v>
-      </c>
-      <c r="AI8" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="AJ8" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="AK8" s="5" t="s">
-        <v>47</v>
       </c>
       <c r="AL8" s="1"/>
     </row>
@@ -1027,7 +1055,9 @@
         <v>27</v>
       </c>
       <c r="AE9" s="4"/>
-      <c r="AF9" s="5"/>
+      <c r="AF9" s="5" t="s">
+        <v>44</v>
+      </c>
       <c r="AG9" s="1"/>
       <c r="AH9" s="1"/>
       <c r="AI9" s="4"/>
@@ -1088,7 +1118,9 @@
         <v>32</v>
       </c>
       <c r="AE10" s="4"/>
-      <c r="AF10" s="5"/>
+      <c r="AF10" s="5" t="s">
+        <v>35</v>
+      </c>
       <c r="AG10" s="1"/>
       <c r="AH10" s="1"/>
       <c r="AI10" s="1"/>
@@ -1638,9 +1670,7 @@
       <c r="O20" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="P20" s="5" t="s">
-        <v>31</v>
-      </c>
+      <c r="P20" s="5"/>
       <c r="Q20" s="5" t="s">
         <v>33</v>
       </c>
@@ -1897,9 +1927,27 @@
       </c>
     </row>
     <row r="28" spans="2:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B28" s="14" t="s">
+      <c r="B28" s="15" t="s">
         <v>1</v>
       </c>
+      <c r="C28" s="16"/>
+      <c r="D28" s="16"/>
+      <c r="E28" s="16"/>
+      <c r="F28" s="16"/>
+      <c r="G28" s="16"/>
+      <c r="H28" s="16"/>
+      <c r="I28" s="16"/>
+      <c r="J28" s="16"/>
+      <c r="K28" s="16"/>
+      <c r="L28" s="16"/>
+      <c r="M28" s="16"/>
+      <c r="N28" s="16"/>
+      <c r="O28" s="16"/>
+      <c r="P28" s="16"/>
+      <c r="Q28" s="16"/>
+      <c r="R28" s="16"/>
+      <c r="S28" s="16"/>
+      <c r="T28" s="16"/>
     </row>
     <row r="29" spans="2:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B29" s="15" t="s">
@@ -2022,22 +2070,92 @@
       <c r="AD32" s="16"/>
       <c r="AE32" s="16"/>
     </row>
-    <row r="33" spans="2:34" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B33" s="14" t="s">
+    <row r="33" spans="2:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B33" s="15" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="34" spans="2:34" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B34" s="14" t="s">
+      <c r="C33" s="16"/>
+      <c r="D33" s="16"/>
+      <c r="E33" s="16"/>
+      <c r="F33" s="16"/>
+      <c r="G33" s="16"/>
+      <c r="H33" s="16"/>
+      <c r="I33" s="16"/>
+      <c r="J33" s="16"/>
+      <c r="K33" s="16"/>
+      <c r="L33" s="16"/>
+      <c r="M33" s="16"/>
+      <c r="N33" s="16"/>
+      <c r="O33" s="16"/>
+      <c r="P33" s="16"/>
+      <c r="Q33" s="16"/>
+      <c r="R33" s="16"/>
+      <c r="S33" s="16"/>
+      <c r="T33" s="16"/>
+      <c r="U33" s="16"/>
+      <c r="V33" s="16"/>
+      <c r="W33" s="16"/>
+      <c r="X33" s="16"/>
+      <c r="Y33" s="16"/>
+      <c r="Z33" s="16"/>
+      <c r="AA33" s="16"/>
+      <c r="AB33" s="16"/>
+      <c r="AC33" s="16"/>
+    </row>
+    <row r="34" spans="2:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B34" s="15" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="35" spans="2:34" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B35" s="14" t="s">
+      <c r="C34" s="16"/>
+      <c r="D34" s="16"/>
+      <c r="E34" s="16"/>
+      <c r="F34" s="16"/>
+      <c r="G34" s="16"/>
+      <c r="H34" s="16"/>
+      <c r="I34" s="16"/>
+    </row>
+    <row r="35" spans="2:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B35" s="15" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="36" spans="2:34" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C35" s="16"/>
+      <c r="D35" s="16"/>
+      <c r="E35" s="16"/>
+      <c r="F35" s="16"/>
+      <c r="G35" s="16"/>
+      <c r="H35" s="16"/>
+      <c r="I35" s="16"/>
+      <c r="J35" s="16"/>
+      <c r="K35" s="16"/>
+      <c r="L35" s="16"/>
+      <c r="M35" s="16"/>
+      <c r="N35" s="16"/>
+      <c r="O35" s="16"/>
+      <c r="P35" s="16"/>
+      <c r="Q35" s="16"/>
+      <c r="R35" s="16"/>
+      <c r="S35" s="16"/>
+      <c r="T35" s="16"/>
+      <c r="U35" s="16"/>
+      <c r="V35" s="16"/>
+      <c r="W35" s="16"/>
+      <c r="X35" s="16"/>
+      <c r="Y35" s="16"/>
+      <c r="Z35" s="16"/>
+      <c r="AA35" s="16"/>
+      <c r="AB35" s="16"/>
+      <c r="AC35" s="16"/>
+      <c r="AD35" s="16"/>
+      <c r="AE35" s="16"/>
+      <c r="AF35" s="16"/>
+      <c r="AG35" s="16"/>
+      <c r="AH35" s="16"/>
+      <c r="AI35" s="16"/>
+      <c r="AJ35" s="16"/>
+      <c r="AK35" s="16"/>
+      <c r="AL35" s="16"/>
+    </row>
+    <row r="36" spans="2:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B36" s="15" t="s">
         <v>9</v>
       </c>
@@ -2055,22 +2173,22 @@
       <c r="N36" s="16"/>
       <c r="O36" s="16"/>
     </row>
-    <row r="37" spans="2:34" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="37" spans="2:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B37" s="14" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="39" spans="2:34" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="39" spans="2:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B39" s="13" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="41" spans="2:34" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="41" spans="2:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B41" s="14" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="42" spans="2:34" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="42" spans="2:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B42" s="15" t="s">
         <v>13</v>
       </c>
@@ -2094,12 +2212,38 @@
       <c r="T42" s="16"/>
       <c r="U42" s="16"/>
     </row>
-    <row r="43" spans="2:34" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B43" s="14" t="s">
+    <row r="43" spans="2:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B43" s="15" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="44" spans="2:34" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C43" s="16"/>
+      <c r="D43" s="16"/>
+      <c r="E43" s="16"/>
+      <c r="F43" s="16"/>
+      <c r="G43" s="16"/>
+      <c r="H43" s="16"/>
+      <c r="I43" s="16"/>
+      <c r="J43" s="16"/>
+      <c r="K43" s="16"/>
+      <c r="L43" s="16"/>
+      <c r="M43" s="16"/>
+      <c r="N43" s="16"/>
+      <c r="O43" s="16"/>
+      <c r="P43" s="16"/>
+      <c r="Q43" s="16"/>
+      <c r="R43" s="16"/>
+      <c r="S43" s="16"/>
+      <c r="T43" s="16"/>
+      <c r="U43" s="16"/>
+      <c r="V43" s="16"/>
+      <c r="W43" s="16"/>
+      <c r="X43" s="16"/>
+      <c r="Y43" s="16"/>
+      <c r="Z43" s="16"/>
+      <c r="AA43" s="16"/>
+      <c r="AB43" s="16"/>
+    </row>
+    <row r="44" spans="2:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B44" s="15" t="s">
         <v>15</v>
       </c>
@@ -2119,7 +2263,7 @@
       <c r="P44" s="16"/>
       <c r="Q44" s="16"/>
     </row>
-    <row r="45" spans="2:34" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="45" spans="2:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B45" s="15" t="s">
         <v>16</v>
       </c>
@@ -2156,12 +2300,12 @@
       <c r="AG45" s="16"/>
       <c r="AH45" s="16"/>
     </row>
-    <row r="46" spans="2:34" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="46" spans="2:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B46" s="14" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="47" spans="2:34" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="47" spans="2:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B47" s="15" t="s">
         <v>18</v>
       </c>
@@ -2184,7 +2328,7 @@
       <c r="S47" s="16"/>
       <c r="T47" s="16"/>
     </row>
-    <row r="48" spans="2:34" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="48" spans="2:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B48" s="15" t="s">
         <v>19</v>
       </c>
@@ -2216,7 +2360,7 @@
       <c r="AB48" s="16"/>
       <c r="AC48" s="16"/>
     </row>
-    <row r="49" spans="2:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="49" spans="2:44" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B49" s="15" t="s">
         <v>20</v>
       </c>
@@ -2244,7 +2388,7 @@
       <c r="X49" s="16"/>
       <c r="Y49" s="16"/>
     </row>
-    <row r="50" spans="2:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="50" spans="2:44" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B50" s="15" t="s">
         <v>21</v>
       </c>
@@ -2272,27 +2416,30 @@
       <c r="X50" s="16"/>
       <c r="Y50" s="16"/>
     </row>
-    <row r="51" spans="2:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="51" spans="2:44" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B51" s="14" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="52" spans="2:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="52" spans="2:44" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B52" s="14" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="53" spans="2:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="AR52" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="53" spans="2:44" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B53" s="14" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="54" spans="2:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="54" spans="2:44" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B54" s="14" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="55" spans="2:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="55" spans="2:44" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B55" s="15" t="s">
         <v>26</v>
       </c>

</xml_diff>